<commit_message>
bilinear interp tests now run
</commit_message>
<xml_diff>
--- a/src/interpolate_test/bilinearInterpExample.xlsx
+++ b/src/interpolate_test/bilinearInterpExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simple-aircraft-simulator\src\interpolate_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62ABD4A6-3DFC-4933-8103-15AA88BFAB3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2540CF-0674-484E-A27F-81E5C2453514}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{72C9D967-7122-4095-9BA9-B780D9B0FF75}"/>
   </bookViews>
@@ -24,12 +24,11 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -67,7 +66,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -387,12 +386,14 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B2" sqref="B2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -445,48 +446,48 @@
         <v>-1</v>
       </c>
       <c r="B2" s="1">
-        <f>EXP(-(B$1^2) -($A2^2))</f>
-        <v>0.1353352832366127</v>
+        <f>EXP(-(B$1^2)+($A2^2))</f>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:L12" si="1">EXP(-(C$1^2) -($A2^2))</f>
-        <v>0.19398004229089189</v>
+        <f t="shared" ref="C2:L12" si="1">EXP(-(C$1^2)+($A2^2))</f>
+        <v>1.4333294145603401</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" si="1"/>
-        <v>0.25666077695355588</v>
+        <v>1.8964808793049512</v>
       </c>
       <c r="E2" s="1">
         <f t="shared" si="1"/>
-        <v>0.31348618088260527</v>
+        <v>2.3163669767810915</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" si="1"/>
-        <v>0.35345468195878016</v>
+        <v>2.6116964734231178</v>
       </c>
       <c r="G2" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144233</v>
+        <v>2.7182818284590451</v>
       </c>
       <c r="H2" s="1">
         <f t="shared" si="1"/>
-        <v>0.35345468195878016</v>
+        <v>2.6116964734231178</v>
       </c>
       <c r="I2" s="1">
         <f t="shared" si="1"/>
-        <v>0.31348618088260527</v>
+        <v>2.3163669767810915</v>
       </c>
       <c r="J2" s="1">
         <f t="shared" si="1"/>
-        <v>0.25666077695355588</v>
+        <v>1.8964808793049512</v>
       </c>
       <c r="K2" s="1">
         <f t="shared" si="1"/>
-        <v>0.19398004229089189</v>
+        <v>1.4333294145603401</v>
       </c>
       <c r="L2" s="1">
         <f t="shared" si="1"/>
-        <v>0.1353352832366127</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -495,48 +496,48 @@
         <v>-0.8</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B12" si="2">EXP(-(B$1^2) -($A3^2))</f>
-        <v>0.19398004229089189</v>
+        <f t="shared" ref="B3:B12" si="2">EXP(-(B$1^2)+($A3^2))</f>
+        <v>0.69767632607103114</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" si="1"/>
-        <v>0.27803730045319408</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144222</v>
+        <v>1.3231298123374369</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" si="1"/>
-        <v>0.44932896411722151</v>
+        <v>1.6160744021928934</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" si="1"/>
-        <v>0.50661699236558955</v>
+        <v>1.8221188003905091</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" si="1"/>
-        <v>0.52729242404304855</v>
+        <v>1.8964808793049517</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" si="1"/>
-        <v>0.50661699236558955</v>
+        <v>1.8221188003905091</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" si="1"/>
-        <v>0.44932896411722151</v>
+        <v>1.6160744021928934</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144222</v>
+        <v>1.3231298123374369</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" si="1"/>
-        <v>0.27803730045319408</v>
+        <v>1</v>
       </c>
       <c r="L3" s="1">
         <f t="shared" si="1"/>
-        <v>0.19398004229089189</v>
+        <v>0.69767632607103114</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -546,47 +547,47 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" si="2"/>
-        <v>0.25666077695355588</v>
+        <v>0.52729242404304866</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144222</v>
+        <v>0.75578374145572547</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>0.48675225595997157</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="1"/>
-        <v>0.59452054797019427</v>
+        <v>1.2214027581601699</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="1"/>
-        <v>0.67032004603563922</v>
+        <v>1.3771277643359572</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="1"/>
-        <v>0.69767632607103103</v>
+        <v>1.4333294145603404</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.67032004603563922</v>
+        <v>1.3771277643359572</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>0.59452054797019427</v>
+        <v>1.2214027581601699</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="1"/>
-        <v>0.48675225595997157</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144222</v>
+        <v>0.75578374145572547</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" si="1"/>
-        <v>0.25666077695355588</v>
+        <v>0.52729242404304866</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -596,47 +597,47 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" si="2"/>
-        <v>0.31348618088260527</v>
+        <v>0.43171052342907973</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="1"/>
-        <v>0.44932896411722151</v>
+        <v>0.61878339180614084</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>0.59452054797019427</v>
+        <v>0.81873075307798182</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="1"/>
-        <v>0.72614903707369083</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
+        <v>1.1274968515793757</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1735108709918103</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1274968515793757</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
         <v>0.81873075307798182</v>
       </c>
-      <c r="G5" s="1">
-        <f t="shared" si="1"/>
-        <v>0.85214378896621124</v>
-      </c>
-      <c r="H5" s="1">
-        <f t="shared" si="1"/>
-        <v>0.81873075307798182</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="1"/>
-        <v>0.72614903707369083</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" si="1"/>
-        <v>0.59452054797019427</v>
-      </c>
       <c r="K5" s="1">
         <f t="shared" si="1"/>
-        <v>0.44932896411722151</v>
+        <v>0.61878339180614084</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="1"/>
-        <v>0.31348618088260527</v>
+        <v>0.43171052342907973</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -646,47 +647,47 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="2"/>
-        <v>0.35345468195878016</v>
+        <v>0.38289288597511206</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
-        <v>0.50661699236558955</v>
+        <v>0.54881163609402639</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>0.67032004603563922</v>
+        <v>0.72614903707369083</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>0.81873075307798182</v>
+        <v>0.88692043671715748</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>0.92311634638663576</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>0.96078943915232318</v>
+        <v>1.0408107741923882</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.92311634638663576</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>0.81873075307798182</v>
+        <v>0.88692043671715748</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
-        <v>0.67032004603563922</v>
+        <v>0.72614903707369083</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="1"/>
-        <v>0.50661699236558955</v>
+        <v>0.54881163609402639</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="1"/>
-        <v>0.35345468195878016</v>
+        <v>0.38289288597511206</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -746,47 +747,47 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="2"/>
-        <v>0.35345468195878016</v>
+        <v>0.38289288597511206</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v>0.50661699236558955</v>
+        <v>0.54881163609402639</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>0.67032004603563922</v>
+        <v>0.72614903707369083</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="1"/>
-        <v>0.81873075307798182</v>
+        <v>0.88692043671715748</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>0.92311634638663576</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>0.96078943915232318</v>
+        <v>1.0408107741923882</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.92311634638663576</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>0.81873075307798182</v>
+        <v>0.88692043671715748</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
-        <v>0.67032004603563922</v>
+        <v>0.72614903707369083</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="1"/>
-        <v>0.50661699236558955</v>
+        <v>0.54881163609402639</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="1"/>
-        <v>0.35345468195878016</v>
+        <v>0.38289288597511206</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -796,47 +797,47 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="2"/>
-        <v>0.31348618088260527</v>
+        <v>0.43171052342907973</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
-        <v>0.44932896411722151</v>
+        <v>0.61878339180614084</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>0.59452054797019427</v>
+        <v>0.81873075307798182</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="1"/>
-        <v>0.72614903707369083</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
+        <v>1.1274968515793757</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1735108709918103</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1274968515793757</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
         <v>0.81873075307798182</v>
       </c>
-      <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.85214378896621135</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.81873075307798182</v>
-      </c>
-      <c r="I9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.72614903707369083</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.59452054797019427</v>
-      </c>
       <c r="K9" s="1">
         <f t="shared" si="1"/>
-        <v>0.44932896411722151</v>
+        <v>0.61878339180614084</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="1"/>
-        <v>0.31348618088260527</v>
+        <v>0.43171052342907973</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -846,47 +847,47 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="2"/>
-        <v>0.25666077695355588</v>
+        <v>0.52729242404304866</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144222</v>
+        <v>0.75578374145572547</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>0.48675225595997157</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="1"/>
-        <v>0.59452054797019427</v>
+        <v>1.2214027581601699</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
-        <v>0.67032004603563922</v>
+        <v>1.3771277643359572</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>0.69767632607103103</v>
+        <v>1.4333294145603404</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
-        <v>0.67032004603563922</v>
+        <v>1.3771277643359572</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>0.59452054797019427</v>
+        <v>1.2214027581601699</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="1"/>
-        <v>0.48675225595997157</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144222</v>
+        <v>0.75578374145572547</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="1"/>
-        <v>0.25666077695355588</v>
+        <v>0.52729242404304866</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -896,47 +897,47 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="2"/>
-        <v>0.19398004229089189</v>
+        <v>0.69767632607103114</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
-        <v>0.27803730045319408</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144222</v>
+        <v>1.3231298123374369</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="1"/>
-        <v>0.44932896411722151</v>
+        <v>1.6160744021928934</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="1"/>
-        <v>0.50661699236558955</v>
+        <v>1.8221188003905091</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>0.52729242404304855</v>
+        <v>1.8964808793049517</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.50661699236558955</v>
+        <v>1.8221188003905091</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>0.44932896411722151</v>
+        <v>1.6160744021928934</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144222</v>
+        <v>1.3231298123374369</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="1"/>
-        <v>0.27803730045319408</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="1"/>
-        <v>0.19398004229089189</v>
+        <v>0.69767632607103114</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -946,47 +947,47 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="2"/>
-        <v>0.1353352832366127</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>0.19398004229089189</v>
+        <v>1.4333294145603401</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>0.25666077695355588</v>
+        <v>1.8964808793049512</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>0.31348618088260527</v>
+        <v>2.3163669767810915</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
-        <v>0.35345468195878016</v>
+        <v>2.6116964734231178</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>0.36787944117144233</v>
+        <v>2.7182818284590451</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.35345468195878016</v>
+        <v>2.6116964734231178</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="1"/>
-        <v>0.31348618088260527</v>
+        <v>2.3163669767810915</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="1"/>
-        <v>0.25666077695355588</v>
+        <v>1.8964808793049512</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="1"/>
-        <v>0.19398004229089189</v>
+        <v>1.4333294145603401</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="1"/>
-        <v>0.1353352832366127</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>